<commit_message>
Error Fix On Contacts Module
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ranvijay\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="4410"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
     <sheet name="deals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>title</t>
   </si>
@@ -42,37 +38,31 @@
     <t>Mr.</t>
   </si>
   <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
     <t>Google</t>
   </si>
   <si>
     <t>Dr.</t>
   </si>
   <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Cris</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
     <t>Mrs.</t>
   </si>
   <si>
-    <t>Mukta</t>
-  </si>
-  <si>
-    <t>Sharma</t>
-  </si>
-  <si>
     <t>Ebay</t>
+  </si>
+  <si>
+    <t>Pooja</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>Anita</t>
+  </si>
+  <si>
+    <t>Ranvijay</t>
   </si>
 </sst>
 </file>
@@ -401,7 +391,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,41 +421,41 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>